<commit_message>
Le programme vérifie si les coordonnées sont correcte et affiche l'emplacement des coordonnées
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00811B6C-2D7D-4852-A6D6-6066568642FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC03506-1C4F-41CF-A338-543AC798BA72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>Finalization de la grille et vérifiquation des coordonnées</t>
+  </si>
+  <si>
+    <t>Faire que le programme vérifie les coordonnée et quil l'affiche</t>
+  </si>
+  <si>
+    <t>Faire une vérification des coordonnées et l'affichage</t>
   </si>
 </sst>
 </file>
@@ -612,7 +618,7 @@
   <dimension ref="E5:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1171,18 +1177,32 @@
       </c>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="9" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
-        <v/>
-      </c>
-      <c r="I24" s="1"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="6"/>
+    <row r="24" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E24" s="4">
+        <v>44265</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="H24" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>4.8611111111111049E-2</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="M24" s="6"/>
     </row>
     <row r="25" spans="5:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
correction de la grille et indication si touché ou à l'eau
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC03506-1C4F-41CF-A338-543AC798BA72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E87F4A0-C7AF-4DF0-BEE9-0DAC4B733A81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>Faire une vérification des coordonnées et l'affichage</t>
+  </si>
+  <si>
+    <t>Correction de bug + rajout de fonctionalité</t>
+  </si>
+  <si>
+    <t>Correction d'érreur d'affichage pour la grille ainsi que vérifier si un bateau ce trouve sur la case des coordonnées et changer l'affichage en correspondance</t>
   </si>
 </sst>
 </file>
@@ -617,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E5:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="D21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1205,18 +1211,32 @@
       </c>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="9" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
-        <v/>
-      </c>
-      <c r="I25" s="1"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="6"/>
+    <row r="25" spans="5:13" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="E25" s="4">
+        <v>44265</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="H25" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="M25" s="6"/>
     </row>
     <row r="26" spans="5:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
rajout de condition de victoire
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E87F4A0-C7AF-4DF0-BEE9-0DAC4B733A81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085C6BBF-B017-4CCE-8C87-E6C4FD633C7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -184,6 +184,18 @@
   </si>
   <si>
     <t>Correction d'érreur d'affichage pour la grille ainsi que vérifier si un bateau ce trouve sur la case des coordonnées et changer l'affichage en correspondance</t>
+  </si>
+  <si>
+    <t>planification</t>
+  </si>
+  <si>
+    <t>Théorie sur les méthode de planification</t>
+  </si>
+  <si>
+    <t>pouvoir gagner</t>
+  </si>
+  <si>
+    <t>Création d'une fonctionqui vérifie si le joueur à terminer la partie</t>
   </si>
 </sst>
 </file>
@@ -623,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E5:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="C21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,7 +649,7 @@
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="15.44140625" customWidth="1"/>
     <col min="11" max="11" width="18.5546875" customWidth="1"/>
-    <col min="12" max="12" width="16.5546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="23.88671875" style="3" customWidth="1"/>
     <col min="13" max="13" width="14" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -693,7 +705,7 @@
       </c>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E7" s="4">
         <v>44238</v>
       </c>
@@ -749,7 +761,7 @@
       </c>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E9" s="4">
         <v>44238</v>
       </c>
@@ -778,7 +790,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E10" s="4">
         <v>44238</v>
       </c>
@@ -807,7 +819,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="5:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E11" s="4">
         <v>44244</v>
       </c>
@@ -837,7 +849,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E12" s="4">
         <v>44244</v>
       </c>
@@ -865,7 +877,7 @@
       </c>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E13" s="4">
         <v>44244</v>
       </c>
@@ -895,7 +907,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="5:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:13" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E14" s="4">
         <v>44244</v>
       </c>
@@ -923,7 +935,7 @@
       </c>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E15" s="4">
         <v>44245</v>
       </c>
@@ -953,7 +965,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="5:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="16" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="E16" s="4">
         <v>44245</v>
       </c>
@@ -983,7 +995,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E17" s="4">
         <v>44245</v>
       </c>
@@ -1011,7 +1023,7 @@
       </c>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="5:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="E18" s="4">
         <v>44246</v>
       </c>
@@ -1041,7 +1053,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="5:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E19" s="4">
         <v>44246</v>
       </c>
@@ -1099,7 +1111,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E21" s="4">
         <v>44260</v>
       </c>
@@ -1127,7 +1139,7 @@
       </c>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E22" s="4">
         <v>44260</v>
       </c>
@@ -1211,7 +1223,7 @@
       </c>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="5:13" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="E25" s="4">
         <v>44265</v>
       </c>
@@ -1239,32 +1251,62 @@
       </c>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="9" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
-        <v/>
-      </c>
-      <c r="I26" s="1"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-    </row>
-    <row r="27" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="9" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
-        <v/>
-      </c>
-      <c r="I27" s="1"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="6"/>
+    <row r="26" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E26" s="4">
+        <v>44266</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="H26" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>2.7777777777777846E-2</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E27" s="4">
+        <v>44266</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H27" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>4.8611111111111105E-2</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="M27" s="6"/>
     </row>
     <row r="28" spans="5:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
résolution d'un bug sur CLion
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8CB1B8-836A-4046-B613-79677E8FD1FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2049AE1E-64D8-40B4-873A-3F557B6C0C4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8160" yWindow="4310" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -647,25 +647,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E5:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="9.08984375" customWidth="1"/>
-    <col min="5" max="5" width="12.36328125" customWidth="1"/>
-    <col min="6" max="6" width="17.6328125" customWidth="1"/>
-    <col min="7" max="7" width="14.6328125" customWidth="1"/>
-    <col min="8" max="8" width="11.90625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="10" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="15.453125" customWidth="1"/>
-    <col min="11" max="11" width="18.54296875" customWidth="1"/>
-    <col min="12" max="12" width="23.90625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" customWidth="1"/>
+    <col min="12" max="12" width="23.88671875" style="3" customWidth="1"/>
     <col min="13" max="13" width="14" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="5:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
@@ -694,7 +694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="5:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E6" s="4">
         <v>44238</v>
       </c>
@@ -717,7 +717,7 @@
       </c>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E7" s="4">
         <v>44238</v>
       </c>
@@ -746,7 +746,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E8" s="4">
         <v>44238</v>
       </c>
@@ -773,7 +773,7 @@
       </c>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E9" s="4">
         <v>44238</v>
       </c>
@@ -802,7 +802,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E10" s="4">
         <v>44238</v>
       </c>
@@ -831,7 +831,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E11" s="4">
         <v>44244</v>
       </c>
@@ -861,7 +861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E12" s="4">
         <v>44244</v>
       </c>
@@ -889,7 +889,7 @@
       </c>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E13" s="4">
         <v>44244</v>
       </c>
@@ -919,7 +919,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="5:13" ht="70.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="5:13" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E14" s="4">
         <v>44244</v>
       </c>
@@ -947,7 +947,7 @@
       </c>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E15" s="4">
         <v>44245</v>
       </c>
@@ -977,7 +977,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="5:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="E16" s="4">
         <v>44245</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E17" s="4">
         <v>44245</v>
       </c>
@@ -1035,7 +1035,7 @@
       </c>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="5:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="E18" s="4">
         <v>44246</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E19" s="4">
         <v>44246</v>
       </c>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="M19" s="6"/>
     </row>
-    <row r="20" spans="5:13" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="5:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="E20" s="4">
         <v>44258</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E21" s="4">
         <v>44260</v>
       </c>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E22" s="4">
         <v>44260</v>
       </c>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="M22" s="6"/>
     </row>
-    <row r="23" spans="5:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="E23" s="4">
         <v>44264</v>
       </c>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="5:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="24" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="E24" s="4">
         <v>44265</v>
       </c>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="5:13" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="5:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="E25" s="4">
         <v>44265</v>
       </c>
@@ -1263,7 +1263,7 @@
       </c>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E26" s="4">
         <v>44266</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="E27" s="4">
         <v>44266</v>
       </c>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="M27" s="6"/>
     </row>
-    <row r="28" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E28" s="4">
         <v>44266</v>
       </c>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E29" s="4">
         <v>44266</v>
       </c>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="M29" s="6"/>
     </row>
-    <row r="30" spans="5:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -1391,7 +1391,7 @@
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
     </row>
-    <row r="31" spans="5:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -1405,7 +1405,7 @@
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
     </row>
-    <row r="32" spans="5:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -1419,7 +1419,7 @@
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
     </row>
-    <row r="33" spans="5:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -1433,7 +1433,7 @@
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
     </row>
-    <row r="34" spans="5:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -1447,7 +1447,7 @@
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
     </row>
-    <row r="35" spans="5:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -1461,7 +1461,7 @@
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
     </row>
-    <row r="36" spans="5:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -1475,7 +1475,7 @@
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="5:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -1489,7 +1489,7 @@
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="5:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -1503,7 +1503,7 @@
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
     </row>
-    <row r="39" spans="5:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -1517,7 +1517,7 @@
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
     </row>
-    <row r="40" spans="5:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>

</xml_diff>

<commit_message>
Rendu le code plus lisible
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2049AE1E-64D8-40B4-873A-3F557B6C0C4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5235B9A2-5C43-4CAD-A0DB-F0EB029091D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -208,6 +208,18 @@
   </si>
   <si>
     <t>ajout d'une option de quitter</t>
+  </si>
+  <si>
+    <t>mise aux propre</t>
+  </si>
+  <si>
+    <t>changement de commentaire, et mise au propre de certaine fonction</t>
+  </si>
+  <si>
+    <t>Résolution de bug</t>
+  </si>
+  <si>
+    <t>obligé l'utilisateur à entré les valeur correctes</t>
   </si>
 </sst>
 </file>
@@ -647,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E5:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1377,32 +1389,60 @@
       </c>
       <c r="M29" s="6"/>
     </row>
-    <row r="30" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="9" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
-        <v/>
-      </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="6"/>
+    <row r="30" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E30" s="4">
+        <v>44267</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0.57986111111111105</v>
+      </c>
+      <c r="H30" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>3.4722222222220989E-3</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="M30" s="6"/>
     </row>
-    <row r="31" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="9" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
-        <v/>
-      </c>
-      <c r="I31" s="1"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="6"/>
+    <row r="31" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E31" s="4">
+        <v>44267</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="H31" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="M31" s="6"/>
     </row>
     <row r="32" spans="5:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Ajout d'un système simple de score, changement léger du menu et ajout d'une "base de donnée"
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A7FDF5-FB70-483B-9DA1-395844320F1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE7D8EC-19E4-4986-A4CC-EED82E34B130}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
   <si>
     <t>Date</t>
   </si>
@@ -226,6 +226,42 @@
   </si>
   <si>
     <t>Réalisation d'une maquette de la bataille navale pour chaque écran</t>
+  </si>
+  <si>
+    <t>organisation</t>
+  </si>
+  <si>
+    <t>Création d'issues sur GitHub et triage des taches</t>
+  </si>
+  <si>
+    <t>recherche</t>
+  </si>
+  <si>
+    <t>trouver comment stocker des valeur dans un fichier et les utilisés dans le programme</t>
+  </si>
+  <si>
+    <t>https://www.programmingsimplified.com/c-program-read-file</t>
+  </si>
+  <si>
+    <t>Implémentation d'une base de donnée</t>
+  </si>
+  <si>
+    <t>Ajout d'un système de base de donnée fonctionnelle ainsi que la lécture des données</t>
+  </si>
+  <si>
+    <t>Modification du menu</t>
+  </si>
+  <si>
+    <t>ajout aux score et à l'authentification dans le menu</t>
+  </si>
+  <si>
+    <t>recherche d'information</t>
+  </si>
+  <si>
+    <t>Ajout du score</t>
+  </si>
+  <si>
+    <t>Ajout d'un système basique de point</t>
   </si>
 </sst>
 </file>
@@ -665,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E5:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1479,74 +1515,148 @@
       </c>
       <c r="M32" s="6"/>
     </row>
-    <row r="33" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="9" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
-        <v/>
-      </c>
-      <c r="I33" s="1"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="6"/>
+    <row r="33" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E33" s="4">
+        <v>44272</v>
+      </c>
+      <c r="F33" s="5">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="H33" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>6.9444444444445308E-3</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="M33" s="6"/>
     </row>
-    <row r="34" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="9" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
-        <v/>
-      </c>
-      <c r="I34" s="1"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-    </row>
-    <row r="35" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="9" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
-        <v/>
-      </c>
-      <c r="I35" s="1"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-    </row>
-    <row r="36" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="9" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
-        <v/>
-      </c>
-      <c r="I36" s="1"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="6"/>
+    <row r="34" spans="5:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="E34" s="4">
+        <v>44272</v>
+      </c>
+      <c r="F34" s="5">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0.57986111111111105</v>
+      </c>
+      <c r="H34" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>3.4722222222220989E-3</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="M34" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="5:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="E35" s="4">
+        <v>44272</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0.57986111111111105</v>
+      </c>
+      <c r="G35" s="5">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="H35" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>1.736111111111116E-2</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E36" s="4">
+        <v>44272</v>
+      </c>
+      <c r="F36" s="5">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="G36" s="5">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="H36" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="9" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
-        <v/>
-      </c>
-      <c r="I37" s="1"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="6"/>
+    <row r="37" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E37" s="4">
+        <v>44272</v>
+      </c>
+      <c r="F37" s="5">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="G37" s="5">
+        <v>0.62152777777777779</v>
+      </c>
+      <c r="H37" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="M37" s="6"/>
     </row>
     <row r="38" spans="5:13" x14ac:dyDescent="0.3">
@@ -1594,11 +1704,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="M34" r:id="rId2" xr:uid="{E9499D6C-6966-4A64-B150-95523B0D59F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commencement d'un scénario de teste et remplissage du journal de travail
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE7D8EC-19E4-4986-A4CC-EED82E34B130}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588CF6D5-7B56-48B6-B1FC-E3654D7AA9CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -262,6 +262,30 @@
   </si>
   <si>
     <t>Ajout d'un système basique de point</t>
+  </si>
+  <si>
+    <t>exercice</t>
+  </si>
+  <si>
+    <t>touver la meilleur manière de tester un jeux</t>
+  </si>
+  <si>
+    <t>Trouver la meilleur manière de tester un jeux tout en parlant en anglais à deux</t>
+  </si>
+  <si>
+    <t>théorie</t>
+  </si>
+  <si>
+    <t>théorie sur les testes</t>
+  </si>
+  <si>
+    <t>Théorie sur les différentes manière de tester un programme</t>
+  </si>
+  <si>
+    <t>Scénario de teste</t>
+  </si>
+  <si>
+    <t>faire un tableau excel pour les scénario de testes</t>
   </si>
 </sst>
 </file>
@@ -701,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E5:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1659,46 +1683,90 @@
       </c>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="9" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
-        <v/>
-      </c>
-      <c r="I38" s="1"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="6"/>
+    <row r="38" spans="5:13" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E38" s="4">
+        <v>44273</v>
+      </c>
+      <c r="F38" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G38" s="5">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="H38" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>80</v>
+      </c>
       <c r="M38" s="6"/>
     </row>
-    <row r="39" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="9" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
-        <v/>
-      </c>
-      <c r="I39" s="1"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-    </row>
-    <row r="40" spans="5:13" x14ac:dyDescent="0.3">
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="9" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
-        <v/>
-      </c>
-      <c r="I40" s="1"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="6"/>
+    <row r="39" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E39" s="4">
+        <v>44273</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="G39" s="5">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="H39" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E40" s="4">
+        <v>44273</v>
+      </c>
+      <c r="F40" s="5">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="H40" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L40" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="M40" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout d'un système de sauvegarde du score
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588CF6D5-7B56-48B6-B1FC-E3654D7AA9CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2098B9F-6E94-4520-9841-ED136D2DA3C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="91">
   <si>
     <t>Date</t>
   </si>
@@ -286,6 +286,23 @@
   </si>
   <si>
     <t>faire un tableau excel pour les scénario de testes</t>
+  </si>
+  <si>
+    <t>Renommer les isseues</t>
+  </si>
+  <si>
+    <t>Rennommer toutes les issues avec la methode smart</t>
+  </si>
+  <si>
+    <t>inscription du score</t>
+  </si>
+  <si>
+    <t>Inscription du score d'un un fichier externe</t>
+  </si>
+  <si>
+    <t>https://www.tutorialspoint.com/c_standard_library/c_function_sp
+rintf.htm
+https://codeforwin.org/2018/02/c-program-append-data-file.html</t>
   </si>
 </sst>
 </file>
@@ -443,8 +460,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M40" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="E5:M40" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M42" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="E5:M42" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Heure Début" dataDxfId="7"/>
@@ -723,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E5:M40"/>
+  <dimension ref="E5:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1769,6 +1786,64 @@
       </c>
       <c r="M40" s="6"/>
     </row>
+    <row r="41" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E41" s="4">
+        <v>44273</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="G41" s="5">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="H41" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="M41" s="6"/>
+    </row>
+    <row r="42" spans="5:13" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="E42" s="4">
+        <v>44274</v>
+      </c>
+      <c r="F42" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="H42" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L42" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M42" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Réalisation de l'écran du score en fonction de la maquette
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2098B9F-6E94-4520-9841-ED136D2DA3C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65F9A0F-A243-40B7-BDB9-DB8EDE35D11B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="94">
   <si>
     <t>Date</t>
   </si>
@@ -303,6 +303,15 @@
     <t>https://www.tutorialspoint.com/c_standard_library/c_function_sp
 rintf.htm
 https://codeforwin.org/2018/02/c-program-append-data-file.html</t>
+  </si>
+  <si>
+    <t>https://www.ltam.lu/cours-c/prg-c42.htm</t>
+  </si>
+  <si>
+    <t>Affichage des scores</t>
+  </si>
+  <si>
+    <t>Réalisation de l'écran des scores en fonction de la maquette</t>
   </si>
 </sst>
 </file>
@@ -460,8 +469,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M42" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="E5:M42" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M43" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="E5:M43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Heure Début" dataDxfId="7"/>
@@ -740,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E5:M42"/>
+  <dimension ref="E5:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+    <sheetView tabSelected="1" topLeftCell="B38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1844,6 +1853,36 @@
         <v>90</v>
       </c>
     </row>
+    <row r="43" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E43" s="4">
+        <v>44279</v>
+      </c>
+      <c r="F43" s="5">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="G43" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="H43" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="M43" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Ajout dans le journal de travail
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65F9A0F-A243-40B7-BDB9-DB8EDE35D11B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59274AA-0818-4025-9021-0BA2ABC7363F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="96">
   <si>
     <t>Date</t>
   </si>
@@ -312,6 +312,12 @@
   </si>
   <si>
     <t>Réalisation de l'écran des scores en fonction de la maquette</t>
+  </si>
+  <si>
+    <t>Faire un dossier de projet par rapport a notre bataille navale</t>
+  </si>
+  <si>
+    <t>Faire un canevas dossier de projet</t>
   </si>
 </sst>
 </file>
@@ -469,8 +475,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M43" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="E5:M43" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M44" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="E5:M44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Heure Début" dataDxfId="7"/>
@@ -749,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E5:M43"/>
+  <dimension ref="E5:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+    <sheetView tabSelected="1" topLeftCell="B41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1883,6 +1889,36 @@
         <v>91</v>
       </c>
     </row>
+    <row r="44" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E44" s="4">
+        <v>44280</v>
+      </c>
+      <c r="F44" s="5">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0.37152777777777773</v>
+      </c>
+      <c r="H44" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L44" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="M44" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Légère modification avec l'affichage des scores
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59274AA-0818-4025-9021-0BA2ABC7363F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6345BB-5043-4CFE-AA01-B17754A765DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -318,6 +318,18 @@
   </si>
   <si>
     <t>Faire un canevas dossier de projet</t>
+  </si>
+  <si>
+    <t>Correction d'un bug</t>
+  </si>
+  <si>
+    <t>Correction du bug faisant crash le programme à la fin de la partie</t>
+  </si>
+  <si>
+    <t>Implémenter une base de donnée de grille</t>
+  </si>
+  <si>
+    <t>Essai d'implémenté les grilles dans les fichiers, pas encore fonctionnel</t>
   </si>
 </sst>
 </file>
@@ -475,8 +487,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M44" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="E5:M44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M46" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="E5:M46" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Heure Début" dataDxfId="7"/>
@@ -755,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E5:M44"/>
+  <dimension ref="E5:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1919,6 +1931,62 @@
         <v>14</v>
       </c>
     </row>
+    <row r="45" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E45" s="4">
+        <v>44280</v>
+      </c>
+      <c r="F45" s="5">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="G45" s="5">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="H45" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>3.4722222222221544E-3</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L45" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="M45" s="6"/>
+    </row>
+    <row r="46" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E46" s="4">
+        <v>44280</v>
+      </c>
+      <c r="F46" s="5">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="G46" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H46" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>3.819444444444442E-2</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="M46" s="6"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Ajout d'un système d'authentification fonctionnelle
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6345BB-5043-4CFE-AA01-B17754A765DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C9813D-1DD6-482B-9D79-B52843A44D01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="105">
   <si>
     <t>Date</t>
   </si>
@@ -330,6 +330,21 @@
   </si>
   <si>
     <t>Essai d'implémenté les grilles dans les fichiers, pas encore fonctionnel</t>
+  </si>
+  <si>
+    <t>Modifier l'affichage des scores</t>
+  </si>
+  <si>
+    <t>Lors de l'enregistrement des scores, l'éspacement va être de telle qu'elle sera aligner avec les en-têtes</t>
+  </si>
+  <si>
+    <t>Ajouter la fonction d'authentification</t>
+  </si>
+  <si>
+    <t>Ajouter l'écran d'authentification, vérification d'érreur et d'enregistrement du nom</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/34108205/reading-the-number-of-characters-in-a-string-in-c/34109568</t>
   </si>
 </sst>
 </file>
@@ -487,8 +502,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M46" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="E5:M46" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M48" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="E5:M48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Heure Début" dataDxfId="7"/>
@@ -767,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E5:M46"/>
+  <dimension ref="E5:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -781,7 +796,7 @@
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
     <col min="8" max="8" width="11.88671875" style="10" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" customWidth="1"/>
     <col min="11" max="11" width="18.5546875" customWidth="1"/>
     <col min="12" max="12" width="23.88671875" style="3" customWidth="1"/>
     <col min="13" max="13" width="14" style="3" customWidth="1"/>
@@ -1986,6 +2001,64 @@
         <v>99</v>
       </c>
       <c r="M46" s="6"/>
+    </row>
+    <row r="47" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E47" s="4">
+        <v>44285</v>
+      </c>
+      <c r="F47" s="5">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="G47" s="5">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="H47" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L47" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="M47" s="6"/>
+    </row>
+    <row r="48" spans="5:13" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="E48" s="4">
+        <v>44285</v>
+      </c>
+      <c r="F48" s="5">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="G48" s="5">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="H48" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L48" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="M48" s="6" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Ajout de deux fonction (pause et afficherLegende) pour garder le code propre et éviter des répétitions
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C9813D-1DD6-482B-9D79-B52843A44D01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721A8F65-7C08-4478-8665-9DEF7F286E46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="107">
   <si>
     <t>Date</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/34108205/reading-the-number-of-characters-in-a-string-in-c/34109568</t>
+  </si>
+  <si>
+    <t>Mettre le nom du joueur avec les scores</t>
+  </si>
+  <si>
+    <t>Lors de l'enregistrement des scores, le nom est enregistrer avec</t>
   </si>
 </sst>
 </file>
@@ -502,8 +508,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M48" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="E5:M48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M49" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="E5:M49" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Heure Début" dataDxfId="7"/>
@@ -782,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E5:M48"/>
+  <dimension ref="E5:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N55" sqref="N55"/>
+      <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2060,6 +2066,34 @@
         <v>104</v>
       </c>
     </row>
+    <row r="49" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E49" s="4">
+        <v>44286</v>
+      </c>
+      <c r="F49" s="5">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="G49" s="5">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="H49" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L49" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M49" s="6"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Création d'une fonction affichant la date et commencement des logs
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721A8F65-7C08-4478-8665-9DEF7F286E46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9A6863-F092-427A-808F-106B7E7BC269}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="110">
   <si>
     <t>Date</t>
   </si>
@@ -351,6 +351,16 @@
   </si>
   <si>
     <t>Lors de l'enregistrement des scores, le nom est enregistrer avec</t>
+  </si>
+  <si>
+    <t>Implémenter une fonction de log</t>
+  </si>
+  <si>
+    <t>Créé un fichier qui enregistre tout les évènement important ainsi que la date et l'heure de l'évènement</t>
+  </si>
+  <si>
+    <t>https://www.studytonight.com/c/programs/misc/display-current-date-and-time
+https://stackoverflow.com/questions/1442116/how-to-get-the-date-and-time-values-in-a-c-program#:~:text=You%20can%20get%20both%20the,time%20and%20date%20in%20UTC.</t>
   </si>
 </sst>
 </file>
@@ -508,8 +518,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M49" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="E5:M49" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M50" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="E5:M50" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Heure Début" dataDxfId="7"/>
@@ -788,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E5:M49"/>
+  <dimension ref="E5:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -805,7 +815,7 @@
     <col min="10" max="10" width="16.109375" customWidth="1"/>
     <col min="11" max="11" width="18.5546875" customWidth="1"/>
     <col min="12" max="12" width="23.88671875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="14" style="3" customWidth="1"/>
+    <col min="13" max="13" width="26.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="5:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1862,7 +1872,7 @@
       </c>
       <c r="M41" s="6"/>
     </row>
-    <row r="42" spans="5:13" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="E42" s="4">
         <v>44274</v>
       </c>
@@ -2036,7 +2046,7 @@
       </c>
       <c r="M47" s="6"/>
     </row>
-    <row r="48" spans="5:13" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="E48" s="4">
         <v>44285</v>
       </c>
@@ -2093,6 +2103,34 @@
         <v>106</v>
       </c>
       <c r="M49" s="6"/>
+    </row>
+    <row r="50" spans="5:13" ht="144" x14ac:dyDescent="0.3">
+      <c r="E50" s="4">
+        <v>44287</v>
+      </c>
+      <c r="F50" s="5">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="G50" s="1"/>
+      <c r="H50" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>-0.34722222222222227</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L50" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="M50" s="6" t="s">
+        <v>109</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Ajout d'un système de log qui enregistre chaque évènement important ainsi que la date et heure
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9A6863-F092-427A-808F-106B7E7BC269}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717FE399-1FC4-43F9-8573-42B95C0C3B06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -360,7 +360,8 @@
   </si>
   <si>
     <t>https://www.studytonight.com/c/programs/misc/display-current-date-and-time
-https://stackoverflow.com/questions/1442116/how-to-get-the-date-and-time-values-in-a-c-program#:~:text=You%20can%20get%20both%20the,time%20and%20date%20in%20UTC.</t>
+https://stackoverflow.com/questions/1442116/how-to-get-the-date-and-time-values-in-a-c-program#:~:text=You%20can%20get%20both%20the,time%20and%20date%20in%20UTC.
+https://www.tutorialspoint.com/cprogramming/c_return_arrays_from_function.htm</t>
   </si>
 </sst>
 </file>
@@ -801,7 +802,7 @@
   <dimension ref="E5:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1246,7 +1247,7 @@
       </c>
       <c r="M19" s="6"/>
     </row>
-    <row r="20" spans="5:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="E20" s="4">
         <v>44258</v>
       </c>
@@ -1642,7 +1643,7 @@
       </c>
       <c r="M33" s="6"/>
     </row>
-    <row r="34" spans="5:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="E34" s="4">
         <v>44272</v>
       </c>
@@ -1672,7 +1673,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="5:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="E35" s="4">
         <v>44272</v>
       </c>
@@ -2104,17 +2105,19 @@
       </c>
       <c r="M49" s="6"/>
     </row>
-    <row r="50" spans="5:13" ht="144" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:13" ht="187.2" x14ac:dyDescent="0.3">
       <c r="E50" s="4">
         <v>44287</v>
       </c>
       <c r="F50" s="5">
         <v>0.34722222222222227</v>
       </c>
-      <c r="G50" s="1"/>
+      <c r="G50" s="5">
+        <v>0.4375</v>
+      </c>
       <c r="H50" s="9">
         <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
-        <v>-0.34722222222222227</v>
+        <v>9.0277777777777735E-2</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Résolution du bug de décalage de la grille
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F09FD48-5482-49D5-99A7-936891903FA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F79CDB-579B-4F62-83C3-C0B50DDE6848}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="125">
   <si>
     <t>Date</t>
   </si>
@@ -402,6 +402,12 @@
   </si>
   <si>
     <t>Corriger un bug</t>
+  </si>
+  <si>
+    <t>Corriger le décalage avec la grille</t>
+  </si>
+  <si>
+    <t>Correction du décalage de 1 avec la grille</t>
   </si>
 </sst>
 </file>
@@ -500,8 +506,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -510,9 +515,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -559,18 +565,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M53" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="E5:M53" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M54" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="E5:M54" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Heure Début" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Heure fin" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Durée" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Type" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Tâche" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Emplacement" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Descriptif" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Source" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Durée" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Type" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Tâche" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Emplacement" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Descriptif" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Source" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -839,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E5:M53"/>
+  <dimension ref="E5:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+      <selection activeCell="L55" sqref="L55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2261,6 +2267,34 @@
       </c>
       <c r="M53" s="6"/>
     </row>
+    <row r="54" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E54" s="4">
+        <v>44287</v>
+      </c>
+      <c r="F54" s="5">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G54" s="5">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="H54" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L54" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="M54" s="6"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Commencement du rapport ainsi d'ajout dans le journal de travail
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F79CDB-579B-4F62-83C3-C0B50DDE6848}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F000C814-7BB6-4C07-B60C-93561634BE69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -847,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E5:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L55" sqref="L55"/>
+    <sheetView tabSelected="1" topLeftCell="D46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Compléter les dernières documentations
</commit_message>
<xml_diff>
--- a/Documentation/JournalDeTravail.xlsx
+++ b/Documentation/JournalDeTravail.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F000C814-7BB6-4C07-B60C-93561634BE69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2793803-98CD-4E00-8A87-B543D1094FBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="130">
   <si>
     <t>Date</t>
   </si>
@@ -408,6 +408,21 @@
   </si>
   <si>
     <t>Correction du décalage de 1 avec la grille</t>
+  </si>
+  <si>
+    <t>Créé un dossier de projet de la bataille navale</t>
+  </si>
+  <si>
+    <t>Création d'un dossier de projet selon l'exemple sur le commun de la classe</t>
+  </si>
+  <si>
+    <t>Faire les testes</t>
+  </si>
+  <si>
+    <t>Donner le projet à Sophie Wäffler pour compléter les testes</t>
+  </si>
+  <si>
+    <t>Donner le projet à Thomas Schwartz pour compléter les testes</t>
   </si>
 </sst>
 </file>
@@ -565,8 +580,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M54" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="E5:M54" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="E5:M57" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="E5:M57" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Heure Début" dataDxfId="7"/>
@@ -845,27 +860,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E5:M54"/>
+  <dimension ref="E5:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="9.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="9.08984375" customWidth="1"/>
+    <col min="5" max="5" width="12.36328125" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" customWidth="1"/>
+    <col min="7" max="7" width="14.6328125" customWidth="1"/>
+    <col min="8" max="8" width="11.90625" style="10" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" customWidth="1"/>
-    <col min="11" max="11" width="18.5546875" customWidth="1"/>
-    <col min="12" max="12" width="23.88671875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="26.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="16.08984375" customWidth="1"/>
+    <col min="11" max="11" width="18.54296875" customWidth="1"/>
+    <col min="12" max="12" width="23.90625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="26.36328125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
@@ -894,7 +909,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E6" s="4">
         <v>44238</v>
       </c>
@@ -917,7 +932,7 @@
       </c>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:13" ht="58" x14ac:dyDescent="0.35">
       <c r="E7" s="4">
         <v>44238</v>
       </c>
@@ -946,7 +961,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E8" s="4">
         <v>44238</v>
       </c>
@@ -973,7 +988,7 @@
       </c>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E9" s="4">
         <v>44238</v>
       </c>
@@ -1002,7 +1017,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E10" s="4">
         <v>44238</v>
       </c>
@@ -1031,7 +1046,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:13" ht="58" x14ac:dyDescent="0.35">
       <c r="E11" s="4">
         <v>44244</v>
       </c>
@@ -1061,7 +1076,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E12" s="4">
         <v>44244</v>
       </c>
@@ -1089,7 +1104,7 @@
       </c>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E13" s="4">
         <v>44244</v>
       </c>
@@ -1119,7 +1134,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="5:13" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:13" ht="70.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E14" s="4">
         <v>44244</v>
       </c>
@@ -1147,7 +1162,7 @@
       </c>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E15" s="4">
         <v>44245</v>
       </c>
@@ -1177,7 +1192,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="5:13" ht="58" x14ac:dyDescent="0.35">
       <c r="E16" s="4">
         <v>44245</v>
       </c>
@@ -1207,7 +1222,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E17" s="4">
         <v>44245</v>
       </c>
@@ -1235,7 +1250,7 @@
       </c>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:13" ht="58" x14ac:dyDescent="0.35">
       <c r="E18" s="4">
         <v>44246</v>
       </c>
@@ -1265,7 +1280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E19" s="4">
         <v>44246</v>
       </c>
@@ -1293,7 +1308,7 @@
       </c>
       <c r="M19" s="6"/>
     </row>
-    <row r="20" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:13" ht="58" x14ac:dyDescent="0.35">
       <c r="E20" s="4">
         <v>44258</v>
       </c>
@@ -1323,7 +1338,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E21" s="4">
         <v>44260</v>
       </c>
@@ -1351,7 +1366,7 @@
       </c>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E22" s="4">
         <v>44260</v>
       </c>
@@ -1379,7 +1394,7 @@
       </c>
       <c r="M22" s="6"/>
     </row>
-    <row r="23" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:13" ht="58" x14ac:dyDescent="0.35">
       <c r="E23" s="4">
         <v>44264</v>
       </c>
@@ -1407,7 +1422,7 @@
       </c>
       <c r="M23" s="6"/>
     </row>
-    <row r="24" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:13" ht="58" x14ac:dyDescent="0.35">
       <c r="E24" s="4">
         <v>44265</v>
       </c>
@@ -1435,7 +1450,7 @@
       </c>
       <c r="M24" s="6"/>
     </row>
-    <row r="25" spans="5:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="E25" s="4">
         <v>44265</v>
       </c>
@@ -1463,7 +1478,7 @@
       </c>
       <c r="M25" s="6"/>
     </row>
-    <row r="26" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:13" ht="29" x14ac:dyDescent="0.35">
       <c r="E26" s="4">
         <v>44266</v>
       </c>
@@ -1493,7 +1508,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E27" s="4">
         <v>44266</v>
       </c>
@@ -1521,7 +1536,7 @@
       </c>
       <c r="M27" s="6"/>
     </row>
-    <row r="28" spans="5:13" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:13" ht="49.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E28" s="4">
         <v>44266</v>
       </c>
@@ -1549,7 +1564,7 @@
       </c>
       <c r="M28" s="6"/>
     </row>
-    <row r="29" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:13" ht="29" x14ac:dyDescent="0.35">
       <c r="E29" s="4">
         <v>44266</v>
       </c>
@@ -1577,7 +1592,7 @@
       </c>
       <c r="M29" s="6"/>
     </row>
-    <row r="30" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E30" s="4">
         <v>44267</v>
       </c>
@@ -1605,7 +1620,7 @@
       </c>
       <c r="M30" s="6"/>
     </row>
-    <row r="31" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E31" s="4">
         <v>44267</v>
       </c>
@@ -1633,7 +1648,7 @@
       </c>
       <c r="M31" s="6"/>
     </row>
-    <row r="32" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E32" s="4">
         <v>44267</v>
       </c>
@@ -1661,7 +1676,7 @@
       </c>
       <c r="M32" s="6"/>
     </row>
-    <row r="33" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E33" s="4">
         <v>44272</v>
       </c>
@@ -1689,7 +1704,7 @@
       </c>
       <c r="M33" s="6"/>
     </row>
-    <row r="34" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:13" ht="58" x14ac:dyDescent="0.35">
       <c r="E34" s="4">
         <v>44272</v>
       </c>
@@ -1719,7 +1734,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:13" ht="58" x14ac:dyDescent="0.35">
       <c r="E35" s="4">
         <v>44272</v>
       </c>
@@ -1749,7 +1764,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E36" s="4">
         <v>44272</v>
       </c>
@@ -1777,7 +1792,7 @@
       </c>
       <c r="M36" s="6"/>
     </row>
-    <row r="37" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:13" ht="29" x14ac:dyDescent="0.35">
       <c r="E37" s="4">
         <v>44272</v>
       </c>
@@ -1805,7 +1820,7 @@
       </c>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="5:13" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:13" ht="60.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E38" s="4">
         <v>44273</v>
       </c>
@@ -1833,7 +1848,7 @@
       </c>
       <c r="M38" s="6"/>
     </row>
-    <row r="39" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E39" s="4">
         <v>44273</v>
       </c>
@@ -1863,7 +1878,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:13" ht="29" x14ac:dyDescent="0.35">
       <c r="E40" s="4">
         <v>44273</v>
       </c>
@@ -1891,7 +1906,7 @@
       </c>
       <c r="M40" s="6"/>
     </row>
-    <row r="41" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E41" s="4">
         <v>44273</v>
       </c>
@@ -1919,7 +1934,7 @@
       </c>
       <c r="M41" s="6"/>
     </row>
-    <row r="42" spans="5:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="E42" s="4">
         <v>44274</v>
       </c>
@@ -1949,7 +1964,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E43" s="4">
         <v>44279</v>
       </c>
@@ -1975,11 +1990,11 @@
       <c r="L43" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="M43" s="6" t="s">
+      <c r="M43" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E44" s="4">
         <v>44280</v>
       </c>
@@ -2009,7 +2024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E45" s="4">
         <v>44280</v>
       </c>
@@ -2037,7 +2052,7 @@
       </c>
       <c r="M45" s="6"/>
     </row>
-    <row r="46" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E46" s="4">
         <v>44280</v>
       </c>
@@ -2065,7 +2080,7 @@
       </c>
       <c r="M46" s="6"/>
     </row>
-    <row r="47" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="5:13" ht="58" x14ac:dyDescent="0.35">
       <c r="E47" s="4">
         <v>44285</v>
       </c>
@@ -2093,7 +2108,7 @@
       </c>
       <c r="M47" s="6"/>
     </row>
-    <row r="48" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="5:13" ht="58" x14ac:dyDescent="0.35">
       <c r="E48" s="4">
         <v>44285</v>
       </c>
@@ -2119,11 +2134,11 @@
       <c r="L48" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="M48" s="6" t="s">
+      <c r="M48" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E49" s="4">
         <v>44286</v>
       </c>
@@ -2151,7 +2166,7 @@
       </c>
       <c r="M49" s="6"/>
     </row>
-    <row r="50" spans="5:13" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:13" ht="188.5" x14ac:dyDescent="0.35">
       <c r="E50" s="4">
         <v>44287</v>
       </c>
@@ -2181,7 +2196,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="5:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="5:13" ht="58" x14ac:dyDescent="0.35">
       <c r="E51" s="4">
         <v>44287</v>
       </c>
@@ -2211,7 +2226,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E52" s="4">
         <v>44287</v>
       </c>
@@ -2239,7 +2254,7 @@
       </c>
       <c r="M52" s="6"/>
     </row>
-    <row r="53" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E53" s="4">
         <v>44287</v>
       </c>
@@ -2267,7 +2282,7 @@
       </c>
       <c r="M53" s="6"/>
     </row>
-    <row r="54" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="E54" s="4">
         <v>44287</v>
       </c>
@@ -2294,16 +2309,102 @@
         <v>124</v>
       </c>
       <c r="M54" s="6"/>
+    </row>
+    <row r="55" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E55" s="4">
+        <v>44288</v>
+      </c>
+      <c r="F55" s="5">
+        <v>0.6875</v>
+      </c>
+      <c r="G55" s="5">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="H55" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L55" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="M55" s="6"/>
+    </row>
+    <row r="56" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E56" s="4">
+        <v>44288</v>
+      </c>
+      <c r="F56" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="G56" s="5">
+        <v>0.8125</v>
+      </c>
+      <c r="H56" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J56" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L56" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="M56" s="6"/>
+    </row>
+    <row r="57" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E57" s="4">
+        <v>44288</v>
+      </c>
+      <c r="F57" s="5">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="G57" s="5">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="H57" s="9">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Heure Début]]),"",Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure Début]])</f>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J57" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L57" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="M57" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="M34" r:id="rId2" xr:uid="{E9499D6C-6966-4A64-B150-95523B0D59F8}"/>
+    <hyperlink ref="M48" r:id="rId3" xr:uid="{DD4FEA58-9BAA-432F-9BE5-256FA0BCC4F4}"/>
+    <hyperlink ref="M43" r:id="rId4" xr:uid="{D7B07BD2-46B0-4B7B-8BFB-DB5E3CEA3C56}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>